<commit_message>
Added new sheet : LoginCredentials
</commit_message>
<xml_diff>
--- a/src/test/resources/UserDetails.xlsx
+++ b/src/test/resources/UserDetails.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22635" windowHeight="7275"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22635" windowHeight="5895" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="credentials" sheetId="1" r:id="rId1"/>
+    <sheet name="UserInformation" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginCredentials" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:M9"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
   <si>
     <t>Password</t>
   </si>
@@ -49,9 +50,6 @@
     <t>abhi@gmail.com</t>
   </si>
   <si>
-    <t>Subha</t>
-  </si>
-  <si>
     <t>subha@yahoo.com</t>
   </si>
   <si>
@@ -86,6 +84,42 @@
   </si>
   <si>
     <t>pup&amp;90</t>
+  </si>
+  <si>
+    <t>Ultimate</t>
+  </si>
+  <si>
+    <t>subha</t>
+  </si>
+  <si>
+    <t>pal</t>
+  </si>
+  <si>
+    <t>tk</t>
+  </si>
+  <si>
+    <t>Rj</t>
+  </si>
+  <si>
+    <t>mohan</t>
+  </si>
+  <si>
+    <t>rj@bksoft.com</t>
+  </si>
+  <si>
+    <t>spdf@*9</t>
+  </si>
+  <si>
+    <t>Sb</t>
+  </si>
+  <si>
+    <t>sb@bksoft.com</t>
+  </si>
+  <si>
+    <t>sb@bk</t>
+  </si>
+  <si>
+    <t>UserName</t>
   </si>
 </sst>
 </file>
@@ -138,10 +172,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -423,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,8 +499,8 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>21</v>
+      <c r="B2" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
@@ -474,33 +514,31 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3">
-        <v>21</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4">
-        <v>21</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" t="s">
         <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
@@ -508,36 +546,67 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5">
-        <v>21</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B6">
-        <v>21</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" t="s">
         <v>20</v>
       </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -548,8 +617,107 @@
     <hyperlink ref="C4" r:id="rId4"/>
     <hyperlink ref="C5" r:id="rId5"/>
     <hyperlink ref="C6" r:id="rId6"/>
+    <hyperlink ref="C7" r:id="rId7"/>
+    <hyperlink ref="D7" r:id="rId8"/>
+    <hyperlink ref="C8" r:id="rId9"/>
+    <hyperlink ref="D8" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="175" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="A5" r:id="rId5"/>
+    <hyperlink ref="A6" r:id="rId6"/>
+    <hyperlink ref="A7" r:id="rId7"/>
+    <hyperlink ref="B7" r:id="rId8"/>
+    <hyperlink ref="A8" r:id="rId9"/>
+    <hyperlink ref="B8" r:id="rId10"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>